<commit_message>
redo results figures and prediction script
</commit_message>
<xml_diff>
--- a/Writing/tables for paper.xlsx
+++ b/Writing/tables for paper.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmgor\Dropbox\Taylor Chapter 3\Predict_Maturity\Writing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5365B5A9-A0C0-48BB-BEF4-087825B3432B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160EDB38-DB8C-4396-9C1C-68E4118D6A9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A492FE8-0195-49DA-881D-9DFBBBF44985}"/>
+    <workbookView xWindow="-28920" yWindow="-1740" windowWidth="29040" windowHeight="15840" xr2:uid="{3A492FE8-0195-49DA-881D-9DFBBBF44985}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="supp tbl 1" sheetId="1" r:id="rId1"/>
+    <sheet name="supp tbl2" sheetId="2" r:id="rId2"/>
+    <sheet name="tbl 1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="162">
   <si>
     <t>Model</t>
   </si>
@@ -172,6 +174,354 @@
   </si>
   <si>
     <t>medium mortality, medium growth</t>
+  </si>
+  <si>
+    <t>Response Variables</t>
+  </si>
+  <si>
+    <t>a50, S</t>
+  </si>
+  <si>
+    <t>Highest R-hat</t>
+  </si>
+  <si>
+    <t>Lmax, Depth, K, Interbirth Interval, Litter Size, Amax, Offspring Size, Trophic Level, Lmat, Temp</t>
+  </si>
+  <si>
+    <t>Convergence</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Lmax, Depth, Interbirth Interval, Litter Size, Amax, Offspring Size, Trophic Level</t>
+  </si>
+  <si>
+    <t>Lmax, Depth, K, Amax, Trophic Level, Temp</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Lmax, Depth, Interbirth Interval, Litter Size, Offspring Size, Trophic Level, Lmat, Temp</t>
+  </si>
+  <si>
+    <t>Lmax, Depth, Interbirth Interval, Litter Size,  Offspring Size, Trophic Level, Lmat, Temp</t>
+  </si>
+  <si>
+    <t>Lmax, Depth, Interbirth Interval, Litter Size, Amax, Offspring Size, Trophic Level, Temp</t>
+  </si>
+  <si>
+    <t>model version for taylor</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Lmax, Depth, Interbirth Interval, Litter Size, Amax, Offspring Size, Trophic Level, Temperature</t>
+  </si>
+  <si>
+    <t>Depth, K, Amax, Trophic Level, Temperature</t>
+  </si>
+  <si>
+    <t>Lmax, Depth, Habitat, Interbirth Interval, Litter Size,  Amax, Offspring Size, Trophic Level, Temperature</t>
+  </si>
+  <si>
+    <t>K, Amax, Trophic Level, Temperature</t>
+  </si>
+  <si>
+    <t>random effects</t>
+  </si>
+  <si>
+    <t>fixed effects</t>
+  </si>
+  <si>
+    <t>model with all covs</t>
+  </si>
+  <si>
+    <t>model with s stripped out, no temp in a50</t>
+  </si>
+  <si>
+    <t>best model</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>best model but fixed effect structure</t>
+  </si>
+  <si>
+    <t>modle with habitat included</t>
+  </si>
+  <si>
+    <t>model with all covs but no VB or age parameters</t>
+  </si>
+  <si>
+    <t>best model no VB or age parameters</t>
+  </si>
+  <si>
+    <t>Lmax, Depth, Interbirth Interval, Litter Size,  Offspring Size, Trophic Level, Temperature</t>
+  </si>
+  <si>
+    <t>Lmax, Depth, Trophic Level, Temperature</t>
+  </si>
+  <si>
+    <t>add prediction model?</t>
+  </si>
+  <si>
+    <t>Transformation of Covariates</t>
+  </si>
+  <si>
+    <t>0-centred</t>
+  </si>
+  <si>
+    <t>mean-centred</t>
+  </si>
+  <si>
+    <t>Scientific Name</t>
+  </si>
+  <si>
+    <t>Common Name</t>
+  </si>
+  <si>
+    <t>Stock Code</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Carcharhinus acronotus</t>
+  </si>
+  <si>
+    <t>BNOS-GOM</t>
+  </si>
+  <si>
+    <t>BNOS-NWA</t>
+  </si>
+  <si>
+    <t>Carcharhinus brachyurus</t>
+  </si>
+  <si>
+    <t>COP-SWA</t>
+  </si>
+  <si>
+    <t>Carcharhinus brevipinna</t>
+  </si>
+  <si>
+    <t>SPIN-WP</t>
+  </si>
+  <si>
+    <t>Carcharhinus cautus</t>
+  </si>
+  <si>
+    <t>NER-I</t>
+  </si>
+  <si>
+    <t>Carcharhinus dussumieri</t>
+  </si>
+  <si>
+    <t>WCH-I</t>
+  </si>
+  <si>
+    <t>Carcharhinus isodon</t>
+  </si>
+  <si>
+    <t>FTH-GOM</t>
+  </si>
+  <si>
+    <t>FTH-NWA</t>
+  </si>
+  <si>
+    <t>Carcharhinus limbatus</t>
+  </si>
+  <si>
+    <t>BTIP-GOM</t>
+  </si>
+  <si>
+    <t>BTIP-NWA</t>
+  </si>
+  <si>
+    <t>Carcharhinus longimanus</t>
+  </si>
+  <si>
+    <t>OCW-WCP</t>
+  </si>
+  <si>
+    <t>Carcharhinus obscurus</t>
+  </si>
+  <si>
+    <t>DUS-NWA</t>
+  </si>
+  <si>
+    <t>Carcharhinus plumbeus</t>
+  </si>
+  <si>
+    <t>SAN-NWA</t>
+  </si>
+  <si>
+    <t>Carcharhinus sorrah</t>
+  </si>
+  <si>
+    <t>SPT-SWP</t>
+  </si>
+  <si>
+    <t>Carcharhinus tilstoni</t>
+  </si>
+  <si>
+    <t>ABTP-SWP</t>
+  </si>
+  <si>
+    <t>Prionace glauca</t>
+  </si>
+  <si>
+    <t>BSH-NWP</t>
+  </si>
+  <si>
+    <t>Rhizoprionodon acutus</t>
+  </si>
+  <si>
+    <t>MLK-I</t>
+  </si>
+  <si>
+    <t>Rhizoprionodon oligolinx</t>
+  </si>
+  <si>
+    <t>GSH-I</t>
+  </si>
+  <si>
+    <t>Rhizoprionodon terraenovae</t>
+  </si>
+  <si>
+    <t>ATSH-NWA</t>
+  </si>
+  <si>
+    <t>ATSH-GOM</t>
+  </si>
+  <si>
+    <t>Scoliodon laticaudus</t>
+  </si>
+  <si>
+    <t>SPD-I</t>
+  </si>
+  <si>
+    <t>Triaenodon obesus</t>
+  </si>
+  <si>
+    <t>WTIP-SWP</t>
+  </si>
+  <si>
+    <t>NMFS 2011</t>
+  </si>
+  <si>
+    <t>NMFS 2007</t>
+  </si>
+  <si>
+    <t>Lucifora 2003</t>
+  </si>
+  <si>
+    <t>Joung 2005</t>
+  </si>
+  <si>
+    <t>Raeisi 2017</t>
+  </si>
+  <si>
+    <t>Carlson 2003</t>
+  </si>
+  <si>
+    <t>Carlson 2005</t>
+  </si>
+  <si>
+    <t>NMFS 2012</t>
+  </si>
+  <si>
+    <t>NMFS 2006</t>
+  </si>
+  <si>
+    <t>WCPO 2012</t>
+  </si>
+  <si>
+    <t>Cortes et al 2006</t>
+  </si>
+  <si>
+    <t>Harry 2013</t>
+  </si>
+  <si>
+    <t>Fujinami 2019</t>
+  </si>
+  <si>
+    <t>Sen 2017</t>
+  </si>
+  <si>
+    <t>Purushottama 2017</t>
+  </si>
+  <si>
+    <t>NMFS 2013</t>
+  </si>
+  <si>
+    <t>Sen 2019</t>
+  </si>
+  <si>
+    <t>Robbins 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year </t>
+  </si>
+  <si>
+    <t>Blacknose shark</t>
+  </si>
+  <si>
+    <t>Bronze whaler</t>
+  </si>
+  <si>
+    <t>Spinner shark</t>
+  </si>
+  <si>
+    <t>Nervous shark</t>
+  </si>
+  <si>
+    <t>Whitecheek shark</t>
+  </si>
+  <si>
+    <t>Finetooth shark</t>
+  </si>
+  <si>
+    <t>Blacktip shark</t>
+  </si>
+  <si>
+    <t>Oceanic whitetip shark</t>
+  </si>
+  <si>
+    <t>Dusky shark</t>
+  </si>
+  <si>
+    <t>Sandbar shark</t>
+  </si>
+  <si>
+    <t>Spottail shark</t>
+  </si>
+  <si>
+    <t>Australian blacktip shark</t>
+  </si>
+  <si>
+    <t>Blue shark</t>
+  </si>
+  <si>
+    <t>Atlantic sharpnose shark</t>
+  </si>
+  <si>
+    <t>Whitetip reef shark</t>
+  </si>
+  <si>
+    <t>Milk shark</t>
+  </si>
+  <si>
+    <t>White 2002</t>
+  </si>
+  <si>
+    <t>Grey sharpnose shark</t>
+  </si>
+  <si>
+    <t>Spadenose shark</t>
   </si>
 </sst>
 </file>
@@ -181,7 +531,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,8 +561,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,8 +604,32 @@
         <bgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor theme="7" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -331,11 +728,103 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -357,11 +846,236 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="6" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="6"/>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -372,6 +1086,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{12D82E99-63B4-417C-96EA-BE9190A4FBC3}" name="Table2" displayName="Table2" ref="K1:O28" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
+  <autoFilter ref="K1:O28" xr:uid="{3D7BBFB4-16C5-4EC4-B959-9A15884C807F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K2:O28">
+    <sortCondition ref="K1:K28"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{7CDB940A-C0D3-4E5F-83CC-C2C22176D177}" name="Scientific Name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{616504E3-DC53-4AC2-A26B-FC901F872F96}" name="Common Name" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{887AF700-D339-4246-892F-9D174BD95A22}" name="Stock Code" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{AA83CEEE-9E2C-491F-B2FE-3116F45F9C75}" name="Year " dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{111BA495-EA9E-42E5-8959-06F29BADD1A5}" name="Source" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -674,7 +1405,7 @@
   <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,9 +1414,10 @@
     <col min="3" max="3" width="12.77734375" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="5.77734375" customWidth="1"/>
-    <col min="11" max="11" width="25.44140625" customWidth="1"/>
+    <col min="11" max="11" width="27.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.33203125" customWidth="1"/>
     <col min="13" max="13" width="29.33203125" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -973,4 +1705,922 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C1D215-1816-4724-9CB5-7F7175988496}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="19">
+        <v>1792</v>
+      </c>
+      <c r="G2" s="19">
+        <v>1.69</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="19">
+        <v>-3364</v>
+      </c>
+      <c r="G3" s="19">
+        <v>1</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="19">
+        <v>1902</v>
+      </c>
+      <c r="G4" s="19">
+        <v>1.83</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="16" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="18">
+        <v>-3365</v>
+      </c>
+      <c r="G5" s="18">
+        <v>1</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="16">
+        <v>33</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="19">
+        <v>0.44</v>
+      </c>
+      <c r="G6" s="19">
+        <v>1.02</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6">
+        <v>20</v>
+      </c>
+      <c r="L6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="19">
+        <v>-3291</v>
+      </c>
+      <c r="G7" s="19">
+        <v>1.03</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7">
+        <v>15</v>
+      </c>
+      <c r="L7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="19">
+        <v>-3366</v>
+      </c>
+      <c r="G8" s="19">
+        <v>1.04</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8">
+        <v>35</v>
+      </c>
+      <c r="L8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="19">
+        <v>-3365</v>
+      </c>
+      <c r="G9" s="19">
+        <v>1.06</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9">
+        <v>34</v>
+      </c>
+      <c r="L9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB93D689-2C6B-4780-B540-63CE92693182}">
+  <dimension ref="A1:T30"/>
+  <sheetViews>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="11" max="11" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.21875" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K1" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="O1" s="45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="K2" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="N2" s="37">
+        <v>2011</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="K3" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="L3" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="M3" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="N3" s="39">
+        <v>2007</v>
+      </c>
+      <c r="O3" s="39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="K4" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="M4" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="N4" s="39">
+        <v>2011</v>
+      </c>
+      <c r="O4" s="39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="K5" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="M5" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="N5" s="37">
+        <v>2003</v>
+      </c>
+      <c r="O5" s="37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="K6" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="M6" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="N6" s="39">
+        <v>2005</v>
+      </c>
+      <c r="O6" s="39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="K7" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="M7" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="N7" s="39">
+        <v>2002</v>
+      </c>
+      <c r="O7" s="39" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="K8" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="L8" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="M8" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="N8" s="37">
+        <v>2017</v>
+      </c>
+      <c r="O8" s="37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="25"/>
+      <c r="C9" s="26"/>
+      <c r="K9" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="L9" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="M9" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="N9" s="37">
+        <v>2003</v>
+      </c>
+      <c r="O9" s="37" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="K10" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="L10" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="M10" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="N10" s="39">
+        <v>2007</v>
+      </c>
+      <c r="O10" s="39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="K11" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="M11" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="N11" s="37">
+        <v>2005</v>
+      </c>
+      <c r="O11" s="37" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="K12" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="L12" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="M12" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="N12" s="37">
+        <v>2012</v>
+      </c>
+      <c r="O12" s="37" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="K13" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="L13" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="M13" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="N13" s="39">
+        <v>2006</v>
+      </c>
+      <c r="O13" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="K14" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="L14" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="M14" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="N14" s="37">
+        <v>2012</v>
+      </c>
+      <c r="O14" s="37" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="K15" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="L15" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="M15" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="N15" s="39">
+        <v>2006</v>
+      </c>
+      <c r="O15" s="39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="K16" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="L16" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="M16" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="N16" s="37">
+        <v>2011</v>
+      </c>
+      <c r="O16" s="37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="29"/>
+      <c r="C17" s="31"/>
+      <c r="K17" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="L17" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="M17" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="N17" s="39">
+        <v>2006</v>
+      </c>
+      <c r="O17" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="27"/>
+      <c r="C18" s="32"/>
+      <c r="K18" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="L18" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="M18" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="N18" s="37">
+        <v>2011</v>
+      </c>
+      <c r="O18" s="37" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="29"/>
+      <c r="C19" s="31"/>
+      <c r="K19" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="L19" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="M19" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="N19" s="37">
+        <v>2013</v>
+      </c>
+      <c r="O19" s="37" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="27"/>
+      <c r="C20" s="28"/>
+      <c r="K20" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="L20" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="M20" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="N20" s="39">
+        <v>2013</v>
+      </c>
+      <c r="O20" s="39" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="29"/>
+      <c r="C21" s="31"/>
+      <c r="K21" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="L21" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="M21" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="N21" s="39">
+        <v>2019</v>
+      </c>
+      <c r="O21" s="39" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="27"/>
+      <c r="C22" s="28"/>
+      <c r="K22" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="L22" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="M22" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="N22" s="39">
+        <v>2017</v>
+      </c>
+      <c r="O22" s="37" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="29"/>
+      <c r="C23" s="31"/>
+      <c r="K23" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="L23" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="M23" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="N23" s="39">
+        <v>2017</v>
+      </c>
+      <c r="O23" s="43" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="K24" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="L24" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="M24" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="N24" s="39">
+        <v>2003</v>
+      </c>
+      <c r="O24" s="39" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="29"/>
+      <c r="C25" s="31"/>
+      <c r="K25" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="L25" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="M25" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="N25" s="37">
+        <v>2007</v>
+      </c>
+      <c r="O25" s="37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="33"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="K26" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="L26" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="M26" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="N26" s="41">
+        <v>2013</v>
+      </c>
+      <c r="O26" s="41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="33"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="K27" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="L27" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="M27" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="N27" s="39">
+        <v>2019</v>
+      </c>
+      <c r="O27" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="33"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="K28" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="L28" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="M28" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="N28" s="42">
+        <v>2006</v>
+      </c>
+      <c r="O28" s="39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="36"/>
+      <c r="R29" s="36"/>
+      <c r="S29" s="36"/>
+      <c r="T29" s="36"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="K30" s="25"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="26"/>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="26"/>
+      <c r="R30" s="26"/>
+      <c r="S30" s="26"/>
+      <c r="T30" s="26"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C25">
+    <sortCondition ref="A2:A25"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>